<commit_message>
updated sfia job spec and the outputs it produces
</commit_message>
<xml_diff>
--- a/outputs/app-pdp-criteria-generator/soft_eng_academy_pdp.xlsx
+++ b/outputs/app-pdp-criteria-generator/soft_eng_academy_pdp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>SkillCode</t>
   </si>
@@ -70,6 +70,21 @@
     <t>Applies newly acquired knowledge to develop new skills</t>
   </si>
   <si>
+    <t>SWDN</t>
+  </si>
+  <si>
+    <t>Creates and documents detailed designs for simple software applications or components</t>
+  </si>
+  <si>
+    <t>Applies agreed modelling techniques, standards, patterns and tools</t>
+  </si>
+  <si>
+    <t>Contributes to the design of components of larger software systems</t>
+  </si>
+  <si>
+    <t>Reviews own work</t>
+  </si>
+  <si>
     <t>PROG</t>
   </si>
   <si>
@@ -79,7 +94,43 @@
     <t>Applies agreed standards and tools to achieve a well-engineered result</t>
   </si>
   <si>
-    <t>Reviews own work</t>
+    <t>SINT</t>
+  </si>
+  <si>
+    <t>Produces software builds from software source code</t>
+  </si>
+  <si>
+    <t>Conducts tests as defined in an integration test specification and records the details of any failures</t>
+  </si>
+  <si>
+    <t>Analyses and reports on integration test activities and results</t>
+  </si>
+  <si>
+    <t>Identifies and reports issues and risks</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Designs test cases, creates test scripts and test data, and automates repeatable tasks working to the requirements or specifications provided</t>
+  </si>
+  <si>
+    <t>Defines test conditions for given requirements</t>
+  </si>
+  <si>
+    <t>Executes and records manual and automated testing  in accordance with test plans</t>
+  </si>
+  <si>
+    <t>Analyses and reports on test activities, results, issues and risks</t>
+  </si>
+  <si>
+    <t>CFMG</t>
+  </si>
+  <si>
+    <t>Applies tools, techniques and processes to administer, track, log, report on and correct configuration items, components and changes</t>
+  </si>
+  <si>
+    <t>Assists with audits to check the accuracy of the information and undertakes any necessary corrective action under direction</t>
   </si>
   <si>
     <t>MADE</t>
@@ -88,13 +139,19 @@
     <t>Example MT</t>
   </si>
   <si>
-    <t>CSOP</t>
-  </si>
-  <si>
-    <t>Processes applications for certification</t>
-  </si>
-  <si>
-    <t>Logs complaints</t>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>Uses standard techniques to elicit, specify, and document requirements for simple subject areas with clearly-defined boundaries</t>
+  </si>
+  <si>
+    <t>Assists in the definition and management of requirements</t>
+  </si>
+  <si>
+    <t>Assists in the creation of a requirements baseline</t>
+  </si>
+  <si>
+    <t>Assists in investigating and applying authorised changes</t>
   </si>
 </sst>
 </file>
@@ -602,28 +659,41 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16"/>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -631,16 +701,227 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
         <v>26</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>